<commit_message>
added functionality of db changing values in DB, names search in export, dialog for detecting newly elibrary ids
</commit_message>
<xml_diff>
--- a/alternative_names.xlsx
+++ b/alternative_names.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>enter_id</t>
   </si>
@@ -28,6 +28,9 @@
     <t>Шустер В.Л., Шустер Владимир Львович</t>
   </si>
   <si>
+    <t>Бобов Д.Г., Бобов Дмитрий Геннадиевич, Бобов Дмитрий Геннадьевич</t>
+  </si>
+  <si>
     <t>Пунанова С.А., Пунанова Светлана Александровна</t>
   </si>
   <si>
@@ -50,9 +53,6 @@
   </si>
   <si>
     <t>Ростовщиков В.Б., Ростовщиков Владимир Борисович</t>
-  </si>
-  <si>
-    <t>Бобов Д.Г., Бобов Дмитрий Геннадиевич, Бобов Дмитрий Геннадьевич</t>
   </si>
   <si>
     <t>Краус З.Т., Краус Зоя Тимофеевна</t>
@@ -419,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -451,7 +451,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>534346</v>
+        <v>6187803222</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -459,7 +459,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>975561</v>
+        <v>534346</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -467,7 +467,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>1090961</v>
+        <v>975561</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -475,7 +475,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>3197441794</v>
+        <v>1090961</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -483,7 +483,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>5383402741</v>
+        <v>3197441794</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>5933130743</v>
+        <v>5383402741</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -499,7 +499,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>7363186540</v>
+        <v>5933130743</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -507,7 +507,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>9811467635</v>
+        <v>7363186540</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -515,7 +515,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>7760348115</v>
+        <v>9811467635</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -523,90 +523,98 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>2109825186</v>
+        <v>7760348115</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>1829979808</v>
+        <v>2109825186</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>2302037906</v>
+        <v>1829979808</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>3870282255</v>
+        <v>2302037906</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>4580834802</v>
+        <v>3870282255</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>5695783741</v>
+        <v>4580834802</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>7700017907</v>
+        <v>5695783741</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>7817442779</v>
+        <v>7700017907</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>8351313473</v>
+        <v>7817442779</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>9880578031</v>
+        <v>8351313473</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
+        <v>9880578031</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
         <v>7633463419</v>
       </c>
-      <c r="B23" t="s">
-        <v>12</v>
+      <c r="B24" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add en-ru recognizer for authors without id, function for adding generated ids to reference table and dialog for handling people with new ids/multiple ids
</commit_message>
<xml_diff>
--- a/alternative_names.xlsx
+++ b/alternative_names.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>enter_id</t>
   </si>
@@ -22,46 +22,58 @@
     <t>new_column_name</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>153485</t>
+  </si>
+  <si>
     <t>Kuklina V., Куклина Вера Владимировна</t>
   </si>
   <si>
     <t>Шустер В.Л., Шустер Владимир Львович</t>
   </si>
   <si>
+    <t>Пунанова С.А., Пунанова Светлана Александровна</t>
+  </si>
+  <si>
+    <t>Kuzmin V.A., Кузьмин В.А.</t>
+  </si>
+  <si>
+    <t>Колоколова И.В., Колоколова Ирина Владимировна</t>
+  </si>
+  <si>
+    <t>Краус З.Т., Краус Зоя Тимофеевна</t>
+  </si>
+  <si>
+    <t>Казанин А.Г., Казанин Алексей Геннадьевич</t>
+  </si>
+  <si>
+    <t>Ростовщиков В.Б., Ростовщиков Владимир Борисович</t>
+  </si>
+  <si>
+    <t>Черных С.П., Черных Сергей Петрович</t>
+  </si>
+  <si>
+    <t>Еременко В.Б., Еременко Василий Борисович</t>
+  </si>
+  <si>
+    <t>Кособреева А.А., Кособреева Александра Александровна</t>
+  </si>
+  <si>
+    <t>Замрий А.В., Замрий Анатолий Владимирович</t>
+  </si>
+  <si>
     <t>Бобов Д.Г., Бобов Дмитрий Геннадиевич, Бобов Дмитрий Геннадьевич</t>
   </si>
   <si>
-    <t>Пунанова С.А., Пунанова Светлана Александровна</t>
-  </si>
-  <si>
-    <t>Казанин А.Г., Казанин Алексей Геннадьевич</t>
-  </si>
-  <si>
-    <t>Колоколова И.В., Колоколова Ирина Владимировна</t>
+    <t>Туманова Е.С., Туманова Екатерина Сергеевна</t>
   </si>
   <si>
     <t>Скворцов А.С., Скворцов Андрей Сергеевич</t>
   </si>
   <si>
-    <t>Черных С.П., Черных Сергей Петрович</t>
-  </si>
-  <si>
-    <t>Туманова Е.С., Туманова Екатерина Сергеевна</t>
-  </si>
-  <si>
-    <t>Еременко В.Б., Еременко Василий Борисович</t>
-  </si>
-  <si>
-    <t>Ростовщиков В.Б., Ростовщиков Владимир Борисович</t>
-  </si>
-  <si>
-    <t>Краус З.Т., Краус Зоя Тимофеевна</t>
-  </si>
-  <si>
-    <t>Кособреева А.А., Кособреева Александра Александровна</t>
-  </si>
-  <si>
-    <t>Замрий А.В., Замрий Анатолий Владимирович</t>
+    <t>Бабич Е.А., Гумерова Р.Р., Еремина И.А., Зарипова Л.Ф., Краус З.Т., Краус Зоя Тимофеевна, Лаптев Ярослав Андреевич, Насекин К.К., Пахомов Андрей Львович, Сейнароев М.Р., Суслов А.А., Фицнер Л.К., Чащина-Семенова О.К.</t>
   </si>
 </sst>
 </file>
@@ -419,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,7 +450,7 @@
         <v>153485</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -446,174 +458,150 @@
         <v>484931</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>6187803222</v>
+        <v>534346</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>534346</v>
+        <v>804891</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>975561</v>
+        <v>1090961</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>1090961</v>
+        <v>9036402995</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>3197441794</v>
+        <v>1487442777</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>5383402741</v>
+        <v>1509268305</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>5933130743</v>
+        <v>2240719343</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>7363186540</v>
+        <v>4006277815</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>9811467635</v>
+        <v>4247549511</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>7760348115</v>
+        <v>4786099333</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>2109825186</v>
+        <v>5945527727</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>1829979808</v>
+        <v>8929086524</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>2302037906</v>
+        <v>9838921473</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>3870282255</v>
+        <v>6893755920</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>4580834802</v>
+        <v>5277594628</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>5695783741</v>
+        <v>6524091593</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20">
-        <v>7700017907</v>
+      <c r="A20" t="s">
+        <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21">
-        <v>7817442779</v>
+      <c r="A21" t="s">
+        <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22">
-        <v>8351313473</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
-        <v>9880578031</v>
-      </c>
-      <c r="B23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24">
-        <v>7633463419</v>
-      </c>
-      <c r="B24" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added functionality for adding alternative ids for people, some changes with interface and function for detecting same people without id with similar ru-en fullnames
</commit_message>
<xml_diff>
--- a/alternative_names.xlsx
+++ b/alternative_names.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>enter_id</t>
   </si>
@@ -22,58 +22,16 @@
     <t>new_column_name</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>153485</t>
-  </si>
-  <si>
-    <t>Kuklina V., Куклина Вера Владимировна</t>
-  </si>
-  <si>
     <t>Шустер В.Л., Шустер Владимир Львович</t>
   </si>
   <si>
     <t>Пунанова С.А., Пунанова Светлана Александровна</t>
   </si>
   <si>
-    <t>Kuzmin V.A., Кузьмин В.А.</t>
-  </si>
-  <si>
     <t>Колоколова И.В., Колоколова Ирина Владимировна</t>
   </si>
   <si>
     <t>Краус З.Т., Краус Зоя Тимофеевна</t>
-  </si>
-  <si>
-    <t>Казанин А.Г., Казанин Алексей Геннадьевич</t>
-  </si>
-  <si>
-    <t>Ростовщиков В.Б., Ростовщиков Владимир Борисович</t>
-  </si>
-  <si>
-    <t>Черных С.П., Черных Сергей Петрович</t>
-  </si>
-  <si>
-    <t>Еременко В.Б., Еременко Василий Борисович</t>
-  </si>
-  <si>
-    <t>Кособреева А.А., Кособреева Александра Александровна</t>
-  </si>
-  <si>
-    <t>Замрий А.В., Замрий Анатолий Владимирович</t>
-  </si>
-  <si>
-    <t>Бобов Д.Г., Бобов Дмитрий Геннадиевич, Бобов Дмитрий Геннадьевич</t>
-  </si>
-  <si>
-    <t>Туманова Е.С., Туманова Екатерина Сергеевна</t>
-  </si>
-  <si>
-    <t>Скворцов А.С., Скворцов Андрей Сергеевич</t>
-  </si>
-  <si>
-    <t>Бабич Е.А., Гумерова Р.Р., Еремина И.А., Зарипова Л.Ф., Краус З.Т., Краус Зоя Тимофеевна, Лаптев Ярослав Андреевич, Насекин К.К., Пахомов Андрей Львович, Сейнароев М.Р., Суслов А.А., Фицнер Л.К., Чащина-Семенова О.К.</t>
   </si>
 </sst>
 </file>
@@ -431,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -447,162 +405,34 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>153485</v>
+        <v>484931</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>484931</v>
+        <v>534346</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>534346</v>
+        <v>1090961</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>804891</v>
+        <v>9036402995</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>1090961</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>9036402995</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>1487442777</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>1509268305</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>2240719343</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>4006277815</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>4247549511</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
-        <v>4786099333</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
-        <v>5945527727</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
-        <v>8929086524</v>
-      </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
-        <v>9838921473</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
-        <v>6893755920</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
-        <v>5277594628</v>
-      </c>
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
-        <v>6524091593</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>